<commit_message>
Update unc-pan-magness to hca-intestine-magness
</commit_message>
<xml_diff>
--- a/staging/hubmap-pancreas_millitome-thompson-2024/resources/lookup2.0.xlsx
+++ b/staging/hubmap-pancreas_millitome-thompson-2024/resources/lookup2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dequeue/Desktop/RUI.nosync/hra-registrations/staging/hubmap-pancreas_millitome-thompson-2024/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728D46D9-49DC-6C42-A058-EB9337A33CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7F4FC4-A6D3-ED43-A6CC-59D4EF13481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5776,12 +5776,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166:C238"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17788,5 +17789,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>